<commit_message>
Added Instructions for Virtual Classroom Exercises.
</commit_message>
<xml_diff>
--- a/Scrum/Classroom/Lesson Plans and Materials/AFS - Session 4/Requirements Backlog Template.xlsx
+++ b/Scrum/Classroom/Lesson Plans and Materials/AFS - Session 4/Requirements Backlog Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732" tabRatio="700" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1. Introduction" sheetId="2" r:id="rId1"/>
@@ -14,10 +14,10 @@
     <sheet name="5.  Retrospective" sheetId="14" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2. Backlog and Planning'!$C$15:$E$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'2. Backlog and Planning'!$B$14</definedName>
     <definedName name="Strongly_Disagree">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
   <si>
     <t>Start</t>
   </si>
@@ -436,11 +436,14 @@
   <si>
     <t>MVP</t>
   </si>
+  <si>
+    <t>Priority</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -598,7 +601,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -669,6 +672,18 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor rgb="FFD3CB8D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -1085,7 +1100,7 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -1400,6 +1415,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1412,15 +1439,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1459,6 +1477,27 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="22" fillId="14" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="22" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1779,7 +1818,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1908,6 +1947,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0B50-4FE6-B4AC-73986C6DF501}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2016,6 +2060,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0B50-4FE6-B4AC-73986C6DF501}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2146,7 +2195,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2217,7 +2265,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2346,6 +2394,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DDF2-4A65-A8F6-EA4878D2A8FA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2454,6 +2507,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DDF2-4A65-A8F6-EA4878D2A8FA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2584,7 +2642,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2655,7 +2712,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2784,6 +2841,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1AF1-4573-B336-43E0A8B2A911}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2892,6 +2954,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1AF1-4573-B336-43E0A8B2A911}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3022,7 +3089,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3093,7 +3159,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3227,6 +3293,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0993-425C-804D-AA7AAD861563}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3276,6 +3347,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0993-425C-804D-AA7AAD861563}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3478,7 +3554,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3602,6 +3678,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DFC0-49DA-AA19-221969108D27}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6735,8 +6816,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B14:G30" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9" headerRowCellStyle="Normal 3">
-  <autoFilter ref="B14:G30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C14:H30" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9" headerRowCellStyle="Normal 3">
+  <autoFilter ref="C14:H30"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Product Release" dataDxfId="8" dataCellStyle="Normal 3 3"/>
     <tableColumn id="2" name="Product Backlog Item" dataDxfId="7" dataCellStyle="Normal 3 3"/>
@@ -7016,90 +7097,90 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" style="3" customWidth="1"/>
-    <col min="2" max="13" width="9.109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.88671875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="2.85546875" style="3" customWidth="1"/>
+    <col min="2" max="13" width="9.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="116"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="165" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="117" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="113"/>
-      <c r="F3" s="113"/>
-      <c r="G3" s="113"/>
-      <c r="H3" s="113"/>
-      <c r="I3" s="113"/>
-      <c r="J3" s="113"/>
-      <c r="K3" s="113"/>
-      <c r="L3" s="113"/>
-      <c r="M3" s="113"/>
-      <c r="N3" s="113"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="117"/>
+      <c r="H3" s="117"/>
+      <c r="I3" s="117"/>
+      <c r="J3" s="117"/>
+      <c r="K3" s="117"/>
+      <c r="L3" s="117"/>
+      <c r="M3" s="117"/>
+      <c r="N3" s="117"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="110"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="110"/>
-      <c r="N4" s="110"/>
-    </row>
-    <row r="5" spans="1:15" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="111" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
+      <c r="N4" s="114"/>
+    </row>
+    <row r="5" spans="1:15" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="115" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="111"/>
-      <c r="L5" s="111"/>
-      <c r="M5" s="111"/>
-      <c r="N5" s="111"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="115"/>
+      <c r="I5" s="115"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
     </row>
   </sheetData>
@@ -7117,64 +7198,78 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O30"/>
+  <dimension ref="A2:P30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" customWidth="1"/>
-    <col min="3" max="3" width="97.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="37" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="89" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" s="19" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="19" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="110" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="115"/>
-      <c r="N2" s="116"/>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="4" spans="1:15" s="19" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="112"/>
+      <c r="P2" s="12"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+    </row>
+    <row r="4" spans="1:16" s="19" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="118" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117"/>
-      <c r="G4" s="117"/>
-      <c r="H4" s="117"/>
-      <c r="I4" s="117"/>
-      <c r="J4" s="117"/>
-      <c r="K4" s="117"/>
-      <c r="L4" s="117"/>
-      <c r="M4" s="117"/>
-      <c r="N4" s="117"/>
-      <c r="O4" s="12"/>
-    </row>
-    <row r="5" spans="1:15" s="19" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="113"/>
+      <c r="M4" s="113"/>
+      <c r="N4" s="113"/>
+      <c r="P4" s="12"/>
+    </row>
+    <row r="5" spans="1:16" s="19" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
-      <c r="B5" s="36"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
       <c r="E5" s="36"/>
@@ -7187,227 +7282,254 @@
       <c r="L5" s="36"/>
       <c r="M5" s="36"/>
       <c r="N5" s="36"/>
-      <c r="O5" s="12"/>
-    </row>
-    <row r="6" spans="1:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="36"/>
+      <c r="P5" s="12"/>
+    </row>
+    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="41"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="41"/>
-    </row>
-    <row r="7" spans="1:15" s="37" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="41"/>
+    </row>
+    <row r="7" spans="1:16" s="37" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="42"/>
-      <c r="C7" s="41"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="41"/>
       <c r="E7" s="41"/>
       <c r="F7" s="41"/>
-    </row>
-    <row r="8" spans="1:15" s="37" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="41"/>
+    </row>
+    <row r="8" spans="1:16" s="37" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="41"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="41"/>
-    </row>
-    <row r="9" spans="1:15" s="37" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="41"/>
+    </row>
+    <row r="9" spans="1:16" s="37" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="42"/>
-      <c r="C9" s="41"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="41"/>
       <c r="E9" s="41"/>
       <c r="F9" s="41"/>
-    </row>
-    <row r="10" spans="1:15" s="37" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="1:16" s="37" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="108"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="41"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="41"/>
-    </row>
-    <row r="11" spans="1:15" s="37" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="41"/>
+    </row>
+    <row r="11" spans="1:16" s="37" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="42"/>
-      <c r="C11" s="109"/>
-      <c r="D11" s="41"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="109"/>
       <c r="E11" s="41"/>
       <c r="F11" s="41"/>
-    </row>
-    <row r="12" spans="1:15" s="37" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="41"/>
+    </row>
+    <row r="12" spans="1:16" s="37" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="108"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="41"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="108"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="41"/>
-    </row>
-    <row r="13" spans="1:15" s="37" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="41"/>
+      <c r="G12" s="41"/>
+    </row>
+    <row r="13" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C13" s="41"/>
       <c r="D13" s="41"/>
       <c r="E13" s="41"/>
       <c r="F13" s="41"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="78" t="s">
+      <c r="G13" s="41"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="131" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="D14" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="79" t="s">
+      <c r="E14" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="79" t="s">
+      <c r="F14" s="79" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="80" t="s">
+      <c r="G14" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="80" t="s">
+      <c r="H14" s="80" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="94"/>
-      <c r="C15" s="99"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="100"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="96"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B16" s="94"/>
-      <c r="C16" s="97"/>
-      <c r="D16" s="98"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="103"/>
-      <c r="G16" s="93"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="94"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="84"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="94"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="84"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="81"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="83"/>
-      <c r="E19" s="104"/>
-      <c r="F19" s="105"/>
-      <c r="G19" s="84"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="81"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="83"/>
-      <c r="E20" s="104"/>
-      <c r="F20" s="105"/>
-      <c r="G20" s="84"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="85"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="105"/>
-      <c r="G21" s="84"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="86"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="104"/>
-      <c r="F22" s="105"/>
-      <c r="G22" s="84"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="86"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="104"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="84"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="86"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="105"/>
-      <c r="G24" s="84"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="86"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="88"/>
-      <c r="E25" s="104"/>
-      <c r="F25" s="105"/>
-      <c r="G25" s="84"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="86"/>
-      <c r="C26" s="87"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="104"/>
-      <c r="F26" s="105"/>
-      <c r="G26" s="84"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="86"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="104"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="84"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="86"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="88"/>
-      <c r="E28" s="104"/>
-      <c r="F28" s="105"/>
-      <c r="G28" s="84"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="86"/>
-      <c r="C29" s="87"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="104"/>
-      <c r="F29" s="105"/>
-      <c r="G29" s="84"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="89"/>
-      <c r="C30" s="90"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="106"/>
-      <c r="F30" s="107"/>
-      <c r="G30" s="92"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="132"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="100"/>
+      <c r="G15" s="101"/>
+      <c r="H15" s="96"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="133"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="93"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="132"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="105"/>
+      <c r="H17" s="84"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="133"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="82"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="104"/>
+      <c r="G18" s="105"/>
+      <c r="H18" s="84"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="134"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="105"/>
+      <c r="H19" s="84"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="135"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="104"/>
+      <c r="G20" s="105"/>
+      <c r="H20" s="84"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="136"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="104"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="84"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="137"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="88"/>
+      <c r="F22" s="104"/>
+      <c r="G22" s="105"/>
+      <c r="H22" s="84"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="136"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="87"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="104"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="84"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="137"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="104"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="84"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="136"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="104"/>
+      <c r="G25" s="105"/>
+      <c r="H25" s="84"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="137"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="88"/>
+      <c r="F26" s="104"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="84"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="136"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="104"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="84"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="137"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="104"/>
+      <c r="G28" s="105"/>
+      <c r="H28" s="84"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="136"/>
+      <c r="C29" s="86"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="104"/>
+      <c r="G29" s="105"/>
+      <c r="H29" s="84"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="137"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="91"/>
+      <c r="F30" s="106"/>
+      <c r="G30" s="107"/>
+      <c r="H30" s="92"/>
     </row>
   </sheetData>
-  <sortState ref="E11:E60">
-    <sortCondition ref="E11:E60" customList="1,2,3"/>
+  <autoFilter ref="B14"/>
+  <sortState ref="F11:F60">
+    <sortCondition ref="F11:F60" customList="1,2,3"/>
   </sortState>
-  <mergeCells count="2">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B4:N4"/>
+  <mergeCells count="1">
+    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7425,48 +7547,48 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="53.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" s="19" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="19" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="121"/>
       <c r="L2" s="12"/>
     </row>
-    <row r="4" spans="1:12" s="19" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="19" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117"/>
-      <c r="G4" s="117"/>
-      <c r="H4" s="117"/>
-      <c r="I4" s="117"/>
-      <c r="J4" s="117"/>
-      <c r="K4" s="117"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="118"/>
+      <c r="I4" s="118"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="1:12" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="19" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="36"/>
       <c r="C5" s="36"/>
@@ -7480,12 +7602,12 @@
       <c r="K5" s="36"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="7" spans="1:12" s="37" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" s="37" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="67" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="40" t="s">
         <v>47</v>
       </c>
@@ -7496,42 +7618,42 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="71"/>
       <c r="C9" s="47"/>
       <c r="D9" s="51"/>
     </row>
-    <row r="10" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="72"/>
       <c r="C10" s="47"/>
       <c r="D10" s="51"/>
     </row>
-    <row r="11" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="73"/>
       <c r="C11" s="47"/>
       <c r="D11" s="51"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="74"/>
       <c r="C12" s="38"/>
       <c r="D12" s="46"/>
     </row>
-    <row r="13" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="75"/>
       <c r="C13" s="38"/>
       <c r="D13" s="46"/>
     </row>
-    <row r="14" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="75"/>
       <c r="C14" s="38"/>
       <c r="D14" s="46"/>
     </row>
-    <row r="15" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="76"/>
       <c r="C15" s="38"/>
       <c r="D15" s="46"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="49"/>
       <c r="C16" s="49"/>
       <c r="D16" s="48"/>
@@ -7539,7 +7661,7 @@
       <c r="F16" s="45"/>
       <c r="G16" s="45"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
       <c r="D17" s="38"/>
@@ -7547,7 +7669,7 @@
       <c r="F17" s="44"/>
       <c r="G17" s="44"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
       <c r="D18" s="48"/>
@@ -7555,7 +7677,7 @@
       <c r="F18" s="44"/>
       <c r="G18" s="44"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
       <c r="D19" s="38"/>
@@ -7563,7 +7685,7 @@
       <c r="F19" s="44"/>
       <c r="G19" s="44"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="50"/>
       <c r="C20" s="50"/>
       <c r="D20" s="52"/>
@@ -7571,7 +7693,7 @@
       <c r="F20" s="45"/>
       <c r="G20" s="45"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="53" t="s">
         <v>31</v>
       </c>
@@ -7584,7 +7706,7 @@
       <c r="F21" s="45"/>
       <c r="G21" s="45"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="53" t="s">
         <v>32</v>
       </c>
@@ -7594,7 +7716,7 @@
       <c r="F22" s="45"/>
       <c r="G22" s="45"/>
     </row>
-    <row r="23" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="54" t="s">
         <v>33</v>
       </c>
@@ -7607,7 +7729,7 @@
       <c r="F23" s="45"/>
       <c r="G23" s="45"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="45"/>
       <c r="C24" s="45"/>
       <c r="D24" s="45"/>
@@ -7615,12 +7737,12 @@
       <c r="F24" s="45"/>
       <c r="G24" s="45"/>
     </row>
-    <row r="25" spans="2:7" s="37" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:7" s="37" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="67" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="2:7" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="40" t="s">
         <v>47</v>
       </c>
@@ -7631,22 +7753,22 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="68"/>
       <c r="C27" s="47"/>
       <c r="D27" s="51"/>
     </row>
-    <row r="28" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="69"/>
       <c r="C28" s="47"/>
       <c r="D28" s="51"/>
     </row>
-    <row r="29" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="70"/>
       <c r="C29" s="47"/>
       <c r="D29" s="51"/>
     </row>
-    <row r="30" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
       <c r="D30" s="38"/>
@@ -7654,7 +7776,7 @@
       <c r="F30" s="44"/>
       <c r="G30" s="44"/>
     </row>
-    <row r="31" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="49"/>
       <c r="C31" s="49"/>
       <c r="D31" s="48"/>
@@ -7662,7 +7784,7 @@
       <c r="F31" s="44"/>
       <c r="G31" s="44"/>
     </row>
-    <row r="32" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
       <c r="D32" s="38"/>
@@ -7670,7 +7792,7 @@
       <c r="F32" s="44"/>
       <c r="G32" s="44"/>
     </row>
-    <row r="33" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="49"/>
       <c r="C33" s="49"/>
       <c r="D33" s="48"/>
@@ -7678,7 +7800,7 @@
       <c r="F33" s="44"/>
       <c r="G33" s="44"/>
     </row>
-    <row r="34" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
       <c r="D34" s="38"/>
@@ -7686,7 +7808,7 @@
       <c r="F34" s="44"/>
       <c r="G34" s="44"/>
     </row>
-    <row r="35" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="50"/>
       <c r="C35" s="50"/>
       <c r="D35" s="48"/>
@@ -7694,7 +7816,7 @@
       <c r="F35" s="45"/>
       <c r="G35" s="45"/>
     </row>
-    <row r="36" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="53" t="s">
         <v>31</v>
       </c>
@@ -7707,7 +7829,7 @@
       <c r="F36" s="45"/>
       <c r="G36" s="45"/>
     </row>
-    <row r="37" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="53" t="s">
         <v>32</v>
       </c>
@@ -7717,7 +7839,7 @@
       <c r="F37" s="45"/>
       <c r="G37" s="45"/>
     </row>
-    <row r="38" spans="2:7" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="54" t="s">
         <v>33</v>
       </c>
@@ -7730,7 +7852,7 @@
       <c r="F38" s="45"/>
       <c r="G38" s="45"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="45"/>
       <c r="C39" s="45"/>
       <c r="D39" s="45"/>
@@ -7738,12 +7860,12 @@
       <c r="F39" s="45"/>
       <c r="G39" s="45"/>
     </row>
-    <row r="40" spans="2:7" s="37" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:7" s="37" customFormat="1" ht="21" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="67" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:7" s="37" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:7" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="40" t="s">
         <v>47</v>
       </c>
@@ -7754,7 +7876,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="49"/>
       <c r="C42" s="49"/>
       <c r="D42" s="48"/>
@@ -7762,7 +7884,7 @@
       <c r="F42" s="45"/>
       <c r="G42" s="45"/>
     </row>
-    <row r="43" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="39"/>
       <c r="C43" s="39"/>
       <c r="D43" s="38"/>
@@ -7770,7 +7892,7 @@
       <c r="F43" s="44"/>
       <c r="G43" s="44"/>
     </row>
-    <row r="44" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="49"/>
       <c r="C44" s="49"/>
       <c r="D44" s="48"/>
@@ -7778,7 +7900,7 @@
       <c r="F44" s="45"/>
       <c r="G44" s="45"/>
     </row>
-    <row r="45" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="39"/>
       <c r="C45" s="39"/>
       <c r="D45" s="38"/>
@@ -7786,7 +7908,7 @@
       <c r="F45" s="44"/>
       <c r="G45" s="44"/>
     </row>
-    <row r="46" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="50"/>
       <c r="C46" s="50"/>
       <c r="D46" s="48"/>
@@ -7794,7 +7916,7 @@
       <c r="F46" s="45"/>
       <c r="G46" s="45"/>
     </row>
-    <row r="47" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="39"/>
       <c r="C47" s="39"/>
       <c r="D47" s="38"/>
@@ -7802,7 +7924,7 @@
       <c r="F47" s="44"/>
       <c r="G47" s="44"/>
     </row>
-    <row r="48" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="49"/>
       <c r="C48" s="49"/>
       <c r="D48" s="48"/>
@@ -7810,7 +7932,7 @@
       <c r="F48" s="45"/>
       <c r="G48" s="45"/>
     </row>
-    <row r="49" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="53" t="s">
         <v>31</v>
       </c>
@@ -7823,7 +7945,7 @@
       <c r="F49" s="45"/>
       <c r="G49" s="45"/>
     </row>
-    <row r="50" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:7" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="53" t="s">
         <v>32</v>
       </c>
@@ -7835,7 +7957,7 @@
       <c r="F50" s="45"/>
       <c r="G50" s="45"/>
     </row>
-    <row r="51" spans="2:7" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:7" s="37" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="54" t="s">
         <v>33</v>
       </c>
@@ -7881,55 +8003,55 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" style="12" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="19" customWidth="1"/>
-    <col min="4" max="5" width="19.88671875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" style="19" customWidth="1"/>
-    <col min="8" max="14" width="9.109375" style="19" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" style="12" customWidth="1"/>
-    <col min="16" max="16384" width="9.109375" style="19"/>
+    <col min="1" max="1" width="2.85546875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="19" customWidth="1"/>
+    <col min="4" max="5" width="19.85546875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="19" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="19" customWidth="1"/>
+    <col min="8" max="14" width="9.140625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="12" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="118" t="s">
+    <row r="1" spans="1:14" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="119" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="119"/>
-      <c r="I2" s="119"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="120"/>
-    </row>
-    <row r="3" spans="1:14" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="117" t="s">
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="121"/>
+    </row>
+    <row r="3" spans="1:14" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="118" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
-      <c r="F3" s="117"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117"/>
-      <c r="I3" s="117"/>
-      <c r="J3" s="117"/>
-      <c r="K3" s="117"/>
-      <c r="L3" s="117"/>
-      <c r="M3" s="117"/>
-      <c r="N3" s="117"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -7944,49 +8066,49 @@
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B6" s="121" t="s">
+    <row r="6" spans="1:14" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="B6" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="121"/>
-      <c r="I6" s="121"/>
-      <c r="J6" s="121"/>
-      <c r="K6" s="121"/>
-      <c r="L6" s="121"/>
-      <c r="M6" s="121"/>
-      <c r="N6" s="121"/>
-    </row>
-    <row r="7" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="122"/>
+      <c r="D6" s="122"/>
+      <c r="E6" s="122"/>
+      <c r="F6" s="122"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="122"/>
+      <c r="L6" s="122"/>
+      <c r="M6" s="122"/>
+      <c r="N6" s="122"/>
+    </row>
+    <row r="7" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
     </row>
-    <row r="8" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="122" t="s">
+    <row r="8" spans="1:14" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B8" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="124"/>
       <c r="E8" s="15">
         <f>'3. Sprint Planning'!D21</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -7996,7 +8118,7 @@
       <c r="M9" s="12"/>
       <c r="N9" s="12"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="22" t="s">
         <v>2</v>
       </c>
@@ -8021,7 +8143,7 @@
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
         <v>0</v>
       </c>
@@ -8041,7 +8163,7 @@
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="14" t="s">
         <v>4</v>
@@ -8065,7 +8187,7 @@
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="14" t="s">
         <v>5</v>
@@ -8089,7 +8211,7 @@
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="14" t="s">
         <v>6</v>
       </c>
@@ -8104,7 +8226,7 @@
       </c>
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="20"/>
       <c r="B15" s="14" t="s">
         <v>7</v>
@@ -8128,7 +8250,7 @@
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
     </row>
-    <row r="16" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="14" t="s">
         <v>8</v>
       </c>
@@ -8143,7 +8265,7 @@
       </c>
       <c r="F16" s="17"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B17" s="14" t="s">
         <v>40</v>
       </c>
@@ -8168,7 +8290,7 @@
       <c r="M17" s="12"/>
       <c r="N17" s="12"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B18" s="14" t="s">
         <v>41</v>
       </c>
@@ -8191,7 +8313,7 @@
       <c r="M18" s="12"/>
       <c r="N18" s="12"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B19" s="14" t="s">
         <v>42</v>
       </c>
@@ -8214,7 +8336,7 @@
       <c r="M19" s="12"/>
       <c r="N19" s="12"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B20" s="14" t="s">
         <v>43</v>
       </c>
@@ -8237,7 +8359,7 @@
       <c r="M20" s="12"/>
       <c r="N20" s="12"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B21" s="14" t="s">
         <v>44</v>
       </c>
@@ -8262,7 +8384,7 @@
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -8272,7 +8394,7 @@
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -8282,48 +8404,48 @@
       <c r="M23" s="12"/>
       <c r="N23" s="12"/>
     </row>
-    <row r="24" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
     </row>
-    <row r="25" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B25" s="121" t="s">
+    <row r="25" spans="1:14" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="B25" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="121"/>
-      <c r="D25" s="121"/>
-      <c r="E25" s="121"/>
-      <c r="F25" s="121"/>
-      <c r="G25" s="121"/>
-      <c r="H25" s="121"/>
-      <c r="I25" s="121"/>
-      <c r="J25" s="121"/>
-      <c r="K25" s="121"/>
-      <c r="L25" s="121"/>
-      <c r="M25" s="121"/>
-      <c r="N25" s="121"/>
-    </row>
-    <row r="26" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="122"/>
+      <c r="D25" s="122"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="122"/>
+      <c r="H25" s="122"/>
+      <c r="I25" s="122"/>
+      <c r="J25" s="122"/>
+      <c r="K25" s="122"/>
+      <c r="L25" s="122"/>
+      <c r="M25" s="122"/>
+      <c r="N25" s="122"/>
+    </row>
+    <row r="26" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
     </row>
-    <row r="27" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="122" t="s">
+    <row r="27" spans="1:14" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B27" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="123"/>
-      <c r="D27" s="123"/>
+      <c r="C27" s="124"/>
+      <c r="D27" s="124"/>
       <c r="E27" s="15">
         <f>'3. Sprint Planning'!D36</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -8333,7 +8455,7 @@
       <c r="M28" s="12"/>
       <c r="N28" s="12"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="B29" s="22" t="s">
         <v>2</v>
       </c>
@@ -8358,7 +8480,7 @@
       <c r="M29" s="12"/>
       <c r="N29" s="12"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B30" s="14" t="s">
         <v>0</v>
       </c>
@@ -8378,7 +8500,7 @@
       <c r="M30" s="12"/>
       <c r="N30" s="12"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="13"/>
       <c r="B31" s="14" t="s">
         <v>4</v>
@@ -8402,7 +8524,7 @@
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="14" t="s">
         <v>5</v>
@@ -8426,7 +8548,7 @@
       <c r="M32" s="12"/>
       <c r="N32" s="12"/>
     </row>
-    <row r="33" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="14" t="s">
         <v>6</v>
       </c>
@@ -8441,7 +8563,7 @@
       </c>
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="20"/>
       <c r="B34" s="14" t="s">
         <v>7</v>
@@ -8465,7 +8587,7 @@
       <c r="M34" s="12"/>
       <c r="N34" s="12"/>
     </row>
-    <row r="35" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B35" s="14" t="s">
         <v>8</v>
       </c>
@@ -8480,7 +8602,7 @@
       </c>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B36" s="14" t="s">
         <v>40</v>
       </c>
@@ -8503,7 +8625,7 @@
       <c r="M36" s="12"/>
       <c r="N36" s="12"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B37" s="14" t="s">
         <v>41</v>
       </c>
@@ -8526,7 +8648,7 @@
       <c r="M37" s="12"/>
       <c r="N37" s="12"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B38" s="14" t="s">
         <v>42</v>
       </c>
@@ -8549,7 +8671,7 @@
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B39" s="14" t="s">
         <v>43</v>
       </c>
@@ -8572,7 +8694,7 @@
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B40" s="14" t="s">
         <v>44</v>
       </c>
@@ -8595,7 +8717,7 @@
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
@@ -8605,41 +8727,41 @@
       <c r="M41" s="12"/>
       <c r="N41" s="12"/>
     </row>
-    <row r="44" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="B44" s="121" t="s">
+    <row r="44" spans="1:14" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="B44" s="122" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="121"/>
-      <c r="D44" s="121"/>
-      <c r="E44" s="121"/>
-      <c r="F44" s="121"/>
-      <c r="G44" s="121"/>
-      <c r="H44" s="121"/>
-      <c r="I44" s="121"/>
-      <c r="J44" s="121"/>
-      <c r="K44" s="121"/>
-      <c r="L44" s="121"/>
-      <c r="M44" s="121"/>
-      <c r="N44" s="121"/>
-    </row>
-    <row r="45" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C44" s="122"/>
+      <c r="D44" s="122"/>
+      <c r="E44" s="122"/>
+      <c r="F44" s="122"/>
+      <c r="G44" s="122"/>
+      <c r="H44" s="122"/>
+      <c r="I44" s="122"/>
+      <c r="J44" s="122"/>
+      <c r="K44" s="122"/>
+      <c r="L44" s="122"/>
+      <c r="M44" s="122"/>
+      <c r="N44" s="122"/>
+    </row>
+    <row r="45" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
       <c r="D45" s="21"/>
       <c r="E45" s="21"/>
       <c r="F45" s="21"/>
     </row>
-    <row r="46" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="122" t="s">
+    <row r="46" spans="1:14" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B46" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="123"/>
-      <c r="D46" s="123"/>
+      <c r="C46" s="124"/>
+      <c r="D46" s="124"/>
       <c r="E46" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
@@ -8649,7 +8771,7 @@
       <c r="M47" s="12"/>
       <c r="N47" s="12"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="B48" s="22" t="s">
         <v>2</v>
       </c>
@@ -8674,7 +8796,7 @@
       <c r="M48" s="12"/>
       <c r="N48" s="12"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B49" s="14" t="s">
         <v>0</v>
       </c>
@@ -8694,7 +8816,7 @@
       <c r="M49" s="12"/>
       <c r="N49" s="12"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="13"/>
       <c r="B50" s="14" t="s">
         <v>4</v>
@@ -8720,7 +8842,7 @@
       <c r="M50" s="12"/>
       <c r="N50" s="12"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="13"/>
       <c r="B51" s="14" t="s">
         <v>5</v>
@@ -8746,7 +8868,7 @@
       <c r="M51" s="12"/>
       <c r="N51" s="12"/>
     </row>
-    <row r="52" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B52" s="14" t="s">
         <v>6</v>
       </c>
@@ -8763,7 +8885,7 @@
       </c>
       <c r="F52" s="17"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="20"/>
       <c r="B53" s="14" t="s">
         <v>7</v>
@@ -8789,7 +8911,7 @@
       <c r="M53" s="12"/>
       <c r="N53" s="12"/>
     </row>
-    <row r="54" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B54" s="14" t="s">
         <v>8</v>
       </c>
@@ -8806,7 +8928,7 @@
       </c>
       <c r="F54" s="17"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B55" s="14" t="s">
         <v>40</v>
       </c>
@@ -8831,7 +8953,7 @@
       <c r="M55" s="12"/>
       <c r="N55" s="12"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B56" s="14" t="s">
         <v>41</v>
       </c>
@@ -8856,7 +8978,7 @@
       <c r="M56" s="12"/>
       <c r="N56" s="12"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B57" s="14" t="s">
         <v>42</v>
       </c>
@@ -8881,7 +9003,7 @@
       <c r="M57" s="12"/>
       <c r="N57" s="12"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B58" s="14" t="s">
         <v>43</v>
       </c>
@@ -8906,7 +9028,7 @@
       <c r="M58" s="12"/>
       <c r="N58" s="12"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B59" s="14" t="s">
         <v>44</v>
       </c>
@@ -8931,7 +9053,7 @@
       <c r="M59" s="12"/>
       <c r="N59" s="12"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G60" s="12"/>
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
@@ -8962,59 +9084,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="50" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleSheetLayoutView="50" workbookViewId="0">
       <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" style="5" customWidth="1"/>
-    <col min="2" max="8" width="30.6640625" style="23" customWidth="1"/>
-    <col min="9" max="10" width="9.109375" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="23"/>
+    <col min="1" max="1" width="2.85546875" style="5" customWidth="1"/>
+    <col min="2" max="8" width="30.7109375" style="23" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="118" t="s">
+    <row r="1" spans="2:8" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
-      <c r="H2" s="120"/>
-    </row>
-    <row r="3" spans="2:8" s="5" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="124" t="s">
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="121"/>
+    </row>
+    <row r="3" spans="2:8" s="5" customFormat="1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="125" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-    </row>
-    <row r="4" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:8" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+    </row>
+    <row r="4" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="2:8" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="124" t="s">
+    <row r="7" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="125" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="124"/>
-      <c r="D8" s="124"/>
-      <c r="E8" s="124"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-    </row>
-    <row r="9" spans="2:8" s="5" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="125"/>
+      <c r="F8" s="125"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+    </row>
+    <row r="9" spans="2:8" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -9023,25 +9145,25 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="129" t="s">
+    <row r="10" spans="2:8" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B10" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="125" t="s">
+      <c r="C10" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="126"/>
-      <c r="E10" s="125" t="s">
+      <c r="D10" s="127"/>
+      <c r="E10" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="126"/>
-      <c r="G10" s="127" t="s">
+      <c r="F10" s="127"/>
+      <c r="G10" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="128"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="129"/>
+      <c r="H10" s="129"/>
+    </row>
+    <row r="11" spans="2:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="B11" s="130"/>
       <c r="C11" s="29" t="s">
         <v>15</v>
       </c>
@@ -9061,7 +9183,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="33" t="s">
         <v>0</v>
       </c>
@@ -9090,7 +9212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="34" t="s">
         <v>4</v>
       </c>
@@ -9119,7 +9241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="34" t="s">
         <v>5</v>
       </c>
@@ -9148,7 +9270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="34" t="s">
         <v>6</v>
       </c>
@@ -9177,7 +9299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="34" t="s">
         <v>7</v>
       </c>
@@ -9206,7 +9328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="34" t="s">
         <v>8</v>
       </c>
@@ -9235,7 +9357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="34" t="s">
         <v>40</v>
       </c>
@@ -9264,7 +9386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="34" t="s">
         <v>41</v>
       </c>
@@ -9293,7 +9415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="34" t="s">
         <v>42</v>
       </c>
@@ -9322,7 +9444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="34" t="s">
         <v>43</v>
       </c>
@@ -9351,7 +9473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="34" t="s">
         <v>44</v>
       </c>
@@ -9380,8 +9502,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="25" t="s">
         <v>16</v>
       </c>
@@ -9410,7 +9532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="35" t="s">
         <v>51</v>
       </c>
@@ -9430,63 +9552,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="24"/>
       <c r="B40" s="24"/>
     </row>
-    <row r="41" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="24"/>
       <c r="B41" s="24"/>
     </row>
-    <row r="42" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="24"/>
       <c r="B42" s="24"/>
     </row>
-    <row r="43" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="24"/>
       <c r="B43" s="24"/>
     </row>
-    <row r="44" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="24"/>
       <c r="B44" s="24"/>
     </row>
-    <row r="45" spans="1:8" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:8" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A45" s="24"/>
       <c r="B45" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="24"/>
       <c r="B46" s="24"/>
     </row>
-    <row r="47" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="24"/>
-      <c r="B47" s="124" t="s">
+      <c r="B47" s="125" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="124"/>
-      <c r="D47" s="124"/>
+      <c r="C47" s="125"/>
+      <c r="D47" s="125"/>
       <c r="E47" s="66"/>
       <c r="F47" s="66"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="1:8" s="5" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="24"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -9496,7 +9618,7 @@
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="1:10" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A49" s="24"/>
       <c r="B49" s="26" t="s">
         <v>18</v>
@@ -9513,7 +9635,7 @@
       <c r="H49" s="5"/>
       <c r="J49" s="23"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B50" s="60"/>
       <c r="C50" s="61"/>
       <c r="D50" s="62"/>
@@ -9523,7 +9645,7 @@
       <c r="H50" s="5"/>
       <c r="J50" s="23"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B51" s="60"/>
       <c r="C51" s="61"/>
       <c r="D51" s="62"/>
@@ -9533,7 +9655,7 @@
       <c r="H51" s="5"/>
       <c r="J51" s="23"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B52" s="60"/>
       <c r="C52" s="61"/>
       <c r="D52" s="62"/>
@@ -9543,7 +9665,7 @@
       <c r="H52" s="5"/>
       <c r="J52" s="23"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B53" s="60"/>
       <c r="C53" s="61"/>
       <c r="D53" s="62"/>
@@ -9553,7 +9675,7 @@
       <c r="H53" s="5"/>
       <c r="J53" s="23"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B54" s="60"/>
       <c r="C54" s="61"/>
       <c r="D54" s="62"/>
@@ -9563,7 +9685,7 @@
       <c r="H54" s="5"/>
       <c r="J54" s="23"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B55" s="60"/>
       <c r="C55" s="61"/>
       <c r="D55" s="62"/>
@@ -9573,7 +9695,7 @@
       <c r="H55" s="5"/>
       <c r="J55" s="23"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B56" s="60"/>
       <c r="C56" s="61"/>
       <c r="D56" s="62"/>
@@ -9583,7 +9705,7 @@
       <c r="H56" s="5"/>
       <c r="J56" s="23"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B57" s="60"/>
       <c r="C57" s="61"/>
       <c r="D57" s="62"/>
@@ -9593,7 +9715,7 @@
       <c r="H57" s="5"/>
       <c r="J57" s="23"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B58" s="60"/>
       <c r="C58" s="61"/>
       <c r="D58" s="62"/>
@@ -9603,7 +9725,7 @@
       <c r="H58" s="5"/>
       <c r="J58" s="23"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B59" s="60"/>
       <c r="C59" s="61"/>
       <c r="D59" s="62"/>
@@ -9613,7 +9735,7 @@
       <c r="H59" s="5"/>
       <c r="J59" s="23"/>
     </row>
-    <row r="60" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B60" s="63"/>
       <c r="C60" s="64"/>
       <c r="D60" s="65"/>
@@ -9623,13 +9745,13 @@
       <c r="H60" s="5"/>
       <c r="J60" s="23"/>
     </row>
-    <row r="61" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B62" s="18"/>
     </row>
-    <row r="63" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="65" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B47:D47"/>
@@ -9648,79 +9770,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <EmailTo xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailHeaders xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <EmailSender xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailFrom xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailSubject xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailCc xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="1104a1b0-c8f6-4ec4-800b-fb1c41b954e8">TQ3A26RQJ2SC-595-25749</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="1104a1b0-c8f6-4ec4-800b-fb1c41b954e8">
-      <Url>http://ilink/its/bps/_layouts/DocIdRedir.aspx?ID=TQ3A26RQJ2SC-595-25749</Url>
-      <Description>TQ3A26RQJ2SC-595-25749</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010002B5E4F0F7BA294A84697710234E31AB" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="08f21f79345a35fc5df453566e973234">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="1104a1b0-c8f6-4ec4-800b-fb1c41b954e8" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5bc494cc63304f0df64b905a1f2ca552" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -9917,41 +9966,80 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B17D183D-DAE7-4098-B303-67DB8FFE16C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1104a1b0-c8f6-4ec4-800b-fb1c41b954e8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0863EC96-2784-49AD-A80E-F4FD02FBBC4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07119253-5AE0-447D-ACD9-80726DC2EAE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <EmailTo xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailHeaders xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <EmailSender xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailFrom xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailSubject xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailCc xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="1104a1b0-c8f6-4ec4-800b-fb1c41b954e8">TQ3A26RQJ2SC-595-25749</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="1104a1b0-c8f6-4ec4-800b-fb1c41b954e8">
+      <Url>http://ilink/its/bps/_layouts/DocIdRedir.aspx?ID=TQ3A26RQJ2SC-595-25749</Url>
+      <Description>TQ3A26RQJ2SC-595-25749</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E512EE9B-A96D-4001-8A60-DCCF81616ED7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9969,4 +10057,38 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07119253-5AE0-447D-ACD9-80726DC2EAE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0863EC96-2784-49AD-A80E-F4FD02FBBC4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B17D183D-DAE7-4098-B303-67DB8FFE16C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1104a1b0-c8f6-4ec4-800b-fb1c41b954e8"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>